<commit_message>
Additional Template Customer Upload
</commit_message>
<xml_diff>
--- a/public/template/Template_Input_Customer.xlsx
+++ b/public/template/Template_Input_Customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadmukhtar/Projects/rpc-be/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB82B7E-052F-E742-843A-F1C7A0CB3727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B0BD28-3DA9-2C4A-B4CC-594E19CFBA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{DABC3E77-F7EC-1A4F-BF20-F0AF2C40BD23}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{DABC3E77-F7EC-1A4F-BF20-F0AF2C40BD23}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,19 @@
     <sheet name="Alamat" sheetId="3" r:id="rId3"/>
     <sheet name="Telepon" sheetId="5" r:id="rId4"/>
     <sheet name="Email" sheetId="4" r:id="rId5"/>
-    <sheet name="Data Gelar" sheetId="6" r:id="rId6"/>
-    <sheet name="Data Grup Pelanggan" sheetId="7" r:id="rId7"/>
-    <sheet name="Data Lokasi" sheetId="8" r:id="rId8"/>
-    <sheet name="Data Kartu Identitas" sheetId="9" r:id="rId9"/>
-    <sheet name="Data Pekerjaan" sheetId="10" r:id="rId10"/>
-    <sheet name="Data Referensi" sheetId="11" r:id="rId11"/>
-    <sheet name="Data Jenis Vet" sheetId="12" r:id="rId12"/>
-    <sheet name="Data Provinsi" sheetId="13" r:id="rId13"/>
-    <sheet name="Data Kabupaten" sheetId="14" r:id="rId14"/>
+    <sheet name="Messenger" sheetId="15" r:id="rId6"/>
+    <sheet name="Data Gelar" sheetId="6" r:id="rId7"/>
+    <sheet name="Data Grup Pelanggan" sheetId="7" r:id="rId8"/>
+    <sheet name="Data Lokasi" sheetId="8" r:id="rId9"/>
+    <sheet name="Data Kartu Identitas" sheetId="9" r:id="rId10"/>
+    <sheet name="Data Pekerjaan" sheetId="10" r:id="rId11"/>
+    <sheet name="Data Referensi" sheetId="11" r:id="rId12"/>
+    <sheet name="Data Jenis Vet" sheetId="12" r:id="rId13"/>
+    <sheet name="Data Provinsi" sheetId="13" r:id="rId14"/>
+    <sheet name="Data Kabupaten" sheetId="14" r:id="rId15"/>
+    <sheet name="Data Kegunaan" sheetId="17" r:id="rId16"/>
+    <sheet name="Data Tipe Telepon" sheetId="18" r:id="rId17"/>
+    <sheet name="Data Tipe Messenger" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -210,24 +214,12 @@
     <t>diisi angka 1 atau 0, jika ya maka disii 0 jika tidak maka diisi 1</t>
   </si>
   <si>
-    <t>Pemakaian</t>
-  </si>
-  <si>
     <t>Alamat Email</t>
   </si>
   <si>
-    <t>Diisi Utama atau Cadangan</t>
-  </si>
-  <si>
     <t>Nomor</t>
   </si>
   <si>
-    <t>Tipe</t>
-  </si>
-  <si>
-    <t>pilihan antara Rumah atau Whatsapp</t>
-  </si>
-  <si>
     <t>Nama Provinsi</t>
   </si>
   <si>
@@ -256,6 +248,36 @@
   </si>
   <si>
     <t>Nomor Member</t>
+  </si>
+  <si>
+    <t>Kode Kegunaan</t>
+  </si>
+  <si>
+    <t>Kegunaan</t>
+  </si>
+  <si>
+    <t>Kode Tipe Telepon</t>
+  </si>
+  <si>
+    <t>Tipe Telepon</t>
+  </si>
+  <si>
+    <t>ID Tipe</t>
+  </si>
+  <si>
+    <t>Menggunakan ID Kegunaan yang ada di sheet Data Kegunaan</t>
+  </si>
+  <si>
+    <t>Menggunakan ID Tipe Telepon yang ada di sheet Data Tipe Telepon</t>
+  </si>
+  <si>
+    <t>ID Pemakaian</t>
+  </si>
+  <si>
+    <t>Nama Akun</t>
+  </si>
+  <si>
+    <t>Kode Messenger</t>
   </si>
 </sst>
 </file>
@@ -704,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -758,7 +780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -817,7 +839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C803CEFE-67A2-744A-9430-E996EF028C1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E9793D-4AC8-2A4A-8AAD-5948094F35C6}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -829,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -838,7 +860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF6DF52-C27B-234B-A597-A62400259554}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C803CEFE-67A2-744A-9430-E996EF028C1F}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -850,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843BC3DC-017E-124A-A244-1AFF9545BE1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF6DF52-C27B-234B-A597-A62400259554}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -871,6 +893,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843BC3DC-017E-124A-A244-1AFF9545BE1C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -879,7 +922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A71B29-7409-E449-9E6A-7608B4CDE4A2}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -896,15 +939,15 @@
         <v>48</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A116C05-EE28-6D4B-A18A-5099B69552C1}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -919,13 +962,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6320BB90-2611-D54C-90F5-0CDA30F71DDB}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7D9512-BA79-004F-83A3-ACE66E397DEF}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752688C6-892A-E04A-9D32-4B1E0C4D97F1}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -937,9 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34951D06-515F-B944-942E-D44029CB5002}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1084,35 +1199,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9973125A-12CB-3342-9B4A-ACC4CAF2042A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1128,6 +1244,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1136,18 +1253,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>55</v>
+      <c r="B2" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="11"/>
     </row>
@@ -1157,6 +1274,47 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E535C28C-8E3E-654D-8B79-6231D4D2BD67}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8648AD32-3A98-004B-81B7-4EA9A958A878}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1172,15 +1330,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD65D569-CA61-7945-8660-52990222D1A0}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1196,15 +1354,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6D5F34-F412-9C4A-9A73-C9CD40A9036D}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1217,28 +1375,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E9793D-4AC8-2A4A-8AAD-5948094F35C6}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>